<commit_message>
Hopefully, 3rd report is finished
</commit_message>
<xml_diff>
--- a/Lab3/3E_tabela.xlsx
+++ b/Lab3/3E_tabela.xlsx
@@ -116,12 +116,20 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -286,17 +294,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>

</xml_diff>